<commit_message>
load site for systems
</commit_message>
<xml_diff>
--- a/lib/criticality/CriticalityData.xlsx
+++ b/lib/criticality/CriticalityData.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majona\Documents\Code\iko_reliability\lib\criticality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3876E2A2-2BC6-4BF6-863A-73EA76F7595D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87289998-2BD6-4101-BD22-905688B47485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{8E9361AC-4A79-4A7B-A1A2-0421436F4C6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E9361AC-4A79-4A7B-A1A2-0421436F4C6B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Systems" sheetId="1" r:id="rId1"/>
+    <sheet name="AssetSystemAssociation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
   <si>
     <t>Safety
 (1-10)</t>
@@ -335,6 +336,9 @@
   </si>
   <si>
     <t>Winders System</t>
+  </si>
+  <si>
+    <t>Siteid</t>
   </si>
 </sst>
 </file>
@@ -390,9 +394,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +434,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -536,7 +540,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -678,7 +682,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05286E0-5DFD-4223-AF84-3CD62AB76C48}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,7 +706,7 @@
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -724,8 +728,11 @@
       <c r="G1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -748,7 +755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -771,7 +778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -794,7 +801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -817,7 +824,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -840,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -863,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -886,7 +893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -909,7 +916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -932,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -955,7 +962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -978,7 +985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2798,4 +2805,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0203A16-3E41-4E06-B004-436557041E79}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>